<commit_message>
First revision of plain type telegram implementation.
</commit_message>
<xml_diff>
--- a/meta/api/BlancoApiSample.xlsx
+++ b/meta/api/BlancoApiSample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/vscode/blanco/blancoRestGeneratorKt/meta/api/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{826A9A8E-3EC4-CC46-BC68-25C648B6E5F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CB3BEB2-642A-0B4D-AFC2-F25AF913F7AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="460" yWindow="500" windowWidth="29440" windowHeight="20500" tabRatio="860" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2440" yWindow="1280" windowWidth="29440" windowHeight="21600" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="process" sheetId="19" r:id="rId1"/>
@@ -2405,12 +2405,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>@io.micronaut.context.annotation.Requirements(
-    io.micronaut.context.annotation.Requires(property = "api-type", value = "sp"),
-)</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>エラー電文(S→C)</t>
     <rPh sb="3" eb="5">
       <t>デンブン</t>
@@ -2633,6 +2627,12 @@
     <rPh sb="0" eb="2">
       <t xml:space="preserve">ツイカ </t>
     </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>@io.micronaut.context.annotation.Requirements(
+    io.micronaut.context.annotation.Requires(property = "api-type", value = "sp")
+)</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -4524,8 +4524,8 @@
   </sheetPr>
   <dimension ref="A1:O75"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45:C47"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -4672,7 +4672,7 @@
       <c r="B14" s="137"/>
       <c r="C14" s="137"/>
       <c r="D14" s="175" t="s">
-        <v>238</v>
+        <v>269</v>
       </c>
       <c r="E14" s="154"/>
     </row>
@@ -5619,7 +5619,7 @@
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D8" s="34"/>
     </row>
@@ -5635,39 +5635,39 @@
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="130" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D10" s="33"/>
       <c r="E10" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="130" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D11" s="33"/>
       <c r="E11" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="46"/>
       <c r="D12" s="33"/>
       <c r="E12" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -6070,7 +6070,7 @@
         <v>116</v>
       </c>
       <c r="I39" s="184" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="J39" s="188" t="s">
         <v>122</v>
@@ -6121,10 +6121,10 @@
         <v>1</v>
       </c>
       <c r="B41" s="56" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C41" s="57" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D41" s="58" t="s">
         <v>102</v>
@@ -6146,10 +6146,10 @@
         <v>2</v>
       </c>
       <c r="B42" s="56" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C42" s="57" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D42" s="58" t="s">
         <v>103</v>
@@ -6701,7 +6701,7 @@
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D8" s="34"/>
     </row>
@@ -6717,39 +6717,39 @@
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="130" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D10" s="33"/>
       <c r="E10" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="130" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D11" s="33"/>
       <c r="E11" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="46"/>
       <c r="D12" s="33"/>
       <c r="E12" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -7152,7 +7152,7 @@
         <v>116</v>
       </c>
       <c r="I39" s="184" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="J39" s="188" t="s">
         <v>122</v>
@@ -7203,10 +7203,10 @@
         <v>1</v>
       </c>
       <c r="B41" s="56" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C41" s="57" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D41" s="58" t="s">
         <v>102</v>
@@ -7228,10 +7228,10 @@
         <v>2</v>
       </c>
       <c r="B42" s="56" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C42" s="57" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D42" s="58" t="s">
         <v>103</v>
@@ -7696,7 +7696,7 @@
   </sheetPr>
   <dimension ref="A1:R67"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I1" sqref="I1:J1048576"/>
     </sheetView>
   </sheetViews>
@@ -7824,13 +7824,13 @@
     </row>
     <row r="13" spans="1:15">
       <c r="A13" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="46"/>
       <c r="D13" s="33"/>
       <c r="E13" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="14" spans="1:15">
@@ -8250,7 +8250,7 @@
     <row r="40" spans="1:18">
       <c r="A40" s="6"/>
       <c r="J40" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="41" spans="1:18">
@@ -8300,10 +8300,10 @@
         <v>116</v>
       </c>
       <c r="I42" s="179" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="J42" s="179" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="K42" s="193" t="s">
         <v>216</v>
@@ -8372,7 +8372,7 @@
       </c>
       <c r="H44" s="23"/>
       <c r="I44" s="23" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="J44" s="123" t="s">
         <v>225</v>
@@ -9095,13 +9095,13 @@
     </row>
     <row r="10" spans="1:15">
       <c r="A10" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="46"/>
       <c r="D10" s="33"/>
       <c r="E10" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -9517,7 +9517,7 @@
         <v>139</v>
       </c>
       <c r="I37" s="184" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="J37" s="179" t="s">
         <v>216</v>
@@ -10165,7 +10165,7 @@
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D8" s="34"/>
     </row>
@@ -10181,39 +10181,39 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="130" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D10" s="33"/>
       <c r="E10" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="130" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D11" s="33"/>
       <c r="E11" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="46"/>
       <c r="D12" s="33"/>
       <c r="E12" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="13" spans="1:14">
@@ -10629,7 +10629,7 @@
         <v>116</v>
       </c>
       <c r="I39" s="192" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="J39" s="179" t="s">
         <v>216</v>
@@ -10684,10 +10684,10 @@
         <v>1</v>
       </c>
       <c r="B41" s="56" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C41" s="57" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D41" s="58" t="s">
         <v>102</v>
@@ -10712,10 +10712,10 @@
         <v>2</v>
       </c>
       <c r="B42" s="56" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C42" s="57" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D42" s="58" t="s">
         <v>103</v>
@@ -11600,7 +11600,7 @@
         <v>229</v>
       </c>
       <c r="H4" s="38" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -11624,7 +11624,7 @@
         <v>230</v>
       </c>
       <c r="H5" s="40" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -11644,12 +11644,12 @@
         <v>228</v>
       </c>
       <c r="H6" s="42" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="41" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B7" s="15"/>
       <c r="C7" s="11" t="s">
@@ -11660,7 +11660,7 @@
       </c>
       <c r="G7" s="129"/>
       <c r="H7" s="11" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -11822,13 +11822,13 @@
     </row>
     <row r="13" spans="1:15">
       <c r="A13" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="46"/>
       <c r="D13" s="33"/>
       <c r="E13" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="14" spans="1:15">
@@ -12248,7 +12248,7 @@
     <row r="40" spans="1:18">
       <c r="A40" s="6"/>
       <c r="J40" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="41" spans="1:18">
@@ -12298,10 +12298,10 @@
         <v>116</v>
       </c>
       <c r="I42" s="179" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="J42" s="179" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="K42" s="179" t="s">
         <v>216</v>
@@ -12368,7 +12368,7 @@
       <c r="G44" s="75"/>
       <c r="H44" s="23"/>
       <c r="I44" s="23" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="J44" s="123" t="s">
         <v>225</v>
@@ -13088,13 +13088,13 @@
     </row>
     <row r="10" spans="1:15">
       <c r="A10" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="46"/>
       <c r="D10" s="33"/>
       <c r="E10" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -13510,7 +13510,7 @@
         <v>116</v>
       </c>
       <c r="I37" s="184" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="J37" s="179" t="s">
         <v>216</v>
@@ -14220,7 +14220,7 @@
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D8" s="34"/>
     </row>
@@ -14236,39 +14236,39 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="130" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D10" s="33"/>
       <c r="E10" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="130" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D11" s="33"/>
       <c r="E11" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="46"/>
       <c r="D12" s="33"/>
       <c r="E12" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="13" spans="1:14">
@@ -14684,7 +14684,7 @@
         <v>116</v>
       </c>
       <c r="I39" s="192" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="J39" s="179" t="s">
         <v>216</v>
@@ -14739,10 +14739,10 @@
         <v>1</v>
       </c>
       <c r="B41" s="56" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C41" s="57" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D41" s="58" t="s">
         <v>102</v>
@@ -14767,10 +14767,10 @@
         <v>2</v>
       </c>
       <c r="B42" s="56" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C42" s="57" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D42" s="58" t="s">
         <v>103</v>
@@ -15265,7 +15265,7 @@
   <dimension ref="A1:R67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J42" sqref="J42:J43"/>
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -15392,13 +15392,13 @@
     </row>
     <row r="13" spans="1:15">
       <c r="A13" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="46"/>
       <c r="D13" s="33"/>
       <c r="E13" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="14" spans="1:15">
@@ -15487,14 +15487,14 @@
     </row>
     <row r="20" spans="1:18">
       <c r="A20" s="113" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B20" s="114"/>
       <c r="C20" s="90" t="s">
+        <v>265</v>
+      </c>
+      <c r="D20" t="s">
         <v>266</v>
-      </c>
-      <c r="D20" t="s">
-        <v>267</v>
       </c>
       <c r="F20"/>
       <c r="G20"/>
@@ -15829,7 +15829,7 @@
     <row r="40" spans="1:18">
       <c r="A40" s="6"/>
       <c r="J40" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="41" spans="1:18">
@@ -15879,10 +15879,10 @@
         <v>116</v>
       </c>
       <c r="I42" s="179" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="J42" s="193" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="K42" s="179" t="s">
         <v>216</v>
@@ -15951,7 +15951,7 @@
       </c>
       <c r="H44" s="23"/>
       <c r="I44" s="23" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="J44" s="123" t="s">
         <v>225</v>
@@ -16674,13 +16674,13 @@
     </row>
     <row r="10" spans="1:15">
       <c r="A10" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="46"/>
       <c r="D10" s="33"/>
       <c r="E10" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -17096,7 +17096,7 @@
         <v>116</v>
       </c>
       <c r="I37" s="184" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="J37" s="179" t="s">
         <v>216</v>
@@ -17808,7 +17808,7 @@
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D8" s="34"/>
     </row>
@@ -17824,37 +17824,37 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="130"/>
       <c r="D10" s="33"/>
       <c r="E10" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="130" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D11" s="33"/>
       <c r="E11" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="46"/>
       <c r="D12" s="33"/>
       <c r="E12" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="13" spans="1:14">
@@ -18270,7 +18270,7 @@
         <v>116</v>
       </c>
       <c r="I39" s="184" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="J39" s="179" t="s">
         <v>216</v>
@@ -18325,10 +18325,10 @@
         <v>1</v>
       </c>
       <c r="B41" s="56" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C41" s="57" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D41" s="58" t="s">
         <v>102</v>
@@ -18353,10 +18353,10 @@
         <v>2</v>
       </c>
       <c r="B42" s="56" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C42" s="57" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D42" s="58" t="s">
         <v>103</v>
@@ -18850,7 +18850,7 @@
   </sheetPr>
   <dimension ref="A1:R67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
@@ -18978,13 +18978,13 @@
     </row>
     <row r="13" spans="1:15">
       <c r="A13" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="46"/>
       <c r="D13" s="33"/>
       <c r="E13" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="14" spans="1:15">
@@ -19071,14 +19071,14 @@
     </row>
     <row r="20" spans="1:18">
       <c r="A20" s="113" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B20" s="114"/>
       <c r="C20" s="90" t="s">
+        <v>265</v>
+      </c>
+      <c r="D20" t="s">
         <v>266</v>
-      </c>
-      <c r="D20" t="s">
-        <v>267</v>
       </c>
       <c r="F20"/>
       <c r="G20"/>
@@ -19415,7 +19415,7 @@
     <row r="40" spans="1:18">
       <c r="A40" s="6"/>
       <c r="J40" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="41" spans="1:18">
@@ -19465,10 +19465,10 @@
         <v>116</v>
       </c>
       <c r="I42" s="179" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="J42" s="193" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="K42" s="179" t="s">
         <v>216</v>
@@ -19537,7 +19537,7 @@
       </c>
       <c r="H44" s="23"/>
       <c r="I44" s="23" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="J44" s="123" t="s">
         <v>225</v>
@@ -20259,13 +20259,13 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="46"/>
       <c r="D10" s="33"/>
       <c r="E10" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -20668,7 +20668,7 @@
         <v>139</v>
       </c>
       <c r="I37" s="184" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="J37" s="188" t="s">
         <v>122</v>

</xml_diff>

<commit_message>
Set NotNull if Nullable is false. Force NotNull to PathVariable query kind.
</commit_message>
<xml_diff>
--- a/meta/api/BlancoApiSample.xlsx
+++ b/meta/api/BlancoApiSample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/vscode/blanco/blancoRestGeneratorKt/meta/api/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CB3BEB2-642A-0B4D-AFC2-F25AF913F7AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D89F724C-83FF-7C49-87BC-1F676D5E5C43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2440" yWindow="1280" windowWidth="29440" windowHeight="21600" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2440" yWindow="1280" windowWidth="29440" windowHeight="21600" tabRatio="860" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="process" sheetId="19" r:id="rId1"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1155" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1152" uniqueCount="270">
   <si>
     <t>項目名</t>
     <rPh sb="0" eb="3">
@@ -4524,8 +4524,8 @@
   </sheetPr>
   <dimension ref="A1:O75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -7696,8 +7696,8 @@
   </sheetPr>
   <dimension ref="A1:R67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:J1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J49" sqref="J49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -8377,9 +8377,7 @@
       <c r="J44" s="123" t="s">
         <v>225</v>
       </c>
-      <c r="K44" s="23" t="s">
-        <v>141</v>
-      </c>
+      <c r="K44" s="23"/>
       <c r="L44" s="23">
         <v>0</v>
       </c>
@@ -11694,7 +11692,7 @@
   <dimension ref="A1:R67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:J1048576"/>
+      <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -12365,7 +12363,9 @@
       </c>
       <c r="E44" s="23"/>
       <c r="F44" s="131"/>
-      <c r="G44" s="75"/>
+      <c r="G44" s="75" t="s">
+        <v>141</v>
+      </c>
       <c r="H44" s="23"/>
       <c r="I44" s="23" t="s">
         <v>257</v>
@@ -12373,9 +12373,7 @@
       <c r="J44" s="123" t="s">
         <v>225</v>
       </c>
-      <c r="K44" s="23" t="s">
-        <v>141</v>
-      </c>
+      <c r="K44" s="23"/>
       <c r="L44" s="23">
         <v>0</v>
       </c>
@@ -15265,7 +15263,7 @@
   <dimension ref="A1:R67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+      <selection activeCell="J47" sqref="J47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -15956,9 +15954,7 @@
       <c r="J44" s="123" t="s">
         <v>225</v>
       </c>
-      <c r="K44" s="23" t="s">
-        <v>141</v>
-      </c>
+      <c r="K44" s="23"/>
       <c r="L44" s="23">
         <v>0</v>
       </c>
@@ -18851,7 +18847,7 @@
   <dimension ref="A1:R67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="J48" sqref="J48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -19542,9 +19538,7 @@
       <c r="J44" s="123" t="s">
         <v>225</v>
       </c>
-      <c r="K44" s="23" t="s">
-        <v>141</v>
-      </c>
+      <c r="K44" s="23"/>
       <c r="L44" s="23">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
3.1.4: always treat query parameters as nullable.
</commit_message>
<xml_diff>
--- a/meta/api/BlancoApiSample.xlsx
+++ b/meta/api/BlancoApiSample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestGeneratorKt/meta/api/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0BFD307-1BEB-ED41-97EF-3699222E88B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80B77192-9906-7746-8DFE-0C94A29A625E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2440" yWindow="500" windowWidth="29440" windowHeight="20500" tabRatio="860" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12760" yWindow="4400" windowWidth="29440" windowHeight="20500" tabRatio="860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="process" sheetId="19" r:id="rId1"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1155" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1152" uniqueCount="270">
   <si>
     <t>項目名</t>
     <rPh sb="0" eb="3">
@@ -11691,8 +11691,8 @@
   </sheetPr>
   <dimension ref="A1:R67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J47" sqref="J47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -12503,9 +12503,7 @@
       <c r="H48" s="25"/>
       <c r="I48" s="25"/>
       <c r="J48" s="123"/>
-      <c r="K48" s="24" t="s">
-        <v>141</v>
-      </c>
+      <c r="K48" s="24"/>
       <c r="L48" s="24"/>
       <c r="M48" s="30"/>
       <c r="N48" s="24"/>
@@ -12533,9 +12531,7 @@
       <c r="H49" s="25"/>
       <c r="I49" s="25"/>
       <c r="J49" s="123"/>
-      <c r="K49" s="24" t="s">
-        <v>141</v>
-      </c>
+      <c r="K49" s="24"/>
       <c r="L49" s="20"/>
       <c r="M49" s="29"/>
       <c r="N49" s="20"/>
@@ -12561,9 +12557,7 @@
       <c r="H50" s="25"/>
       <c r="I50" s="25"/>
       <c r="J50" s="123"/>
-      <c r="K50" s="24" t="s">
-        <v>141</v>
-      </c>
+      <c r="K50" s="24"/>
       <c r="L50" s="20"/>
       <c r="M50" s="29"/>
       <c r="N50" s="20"/>
@@ -15264,8 +15258,8 @@
   </sheetPr>
   <dimension ref="A1:R67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J49" sqref="J49"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>

</xml_diff>